<commit_message>
I fixed the Turnover and OES Report CSV files; previously, they were not opening probably here. But, I was able to fix them in Excel and readd them here
</commit_message>
<xml_diff>
--- a/OES_Report.xlsx
+++ b/OES_Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncorw\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncorw\Documents\School\2024\Fall\Data Tech Analytics\Week 3\final-project-cortesne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E603685B-8D7B-457C-869D-4AF6A758C6A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E4ECFB-B534-4A1A-8D58-A303380A6FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14820" yWindow="2235" windowWidth="21180" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OES Sheet" sheetId="1" r:id="rId1"/>
@@ -833,17 +833,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -868,23 +864,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -906,18 +891,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1252,879 +1233,866 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="A24:C32"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="16" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+    <row r="1" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+    <row r="2" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+    <row r="3" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>15</v>
+    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>43</v>
+        <v>116</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>44</v>
+        <v>117</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>51</v>
+        <v>125</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>44</v>
+        <v>133</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>56</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>57</v>
+        <v>137</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>63</v>
+        <v>142</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>64</v>
+        <v>143</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>65</v>
+        <v>144</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>72</v>
+        <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>73</v>
+        <v>152</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>138</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>76</v>
+        <v>139</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>82</v>
+        <v>145</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>83</v>
+        <v>146</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>84</v>
+        <v>147</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>85</v>
+        <v>148</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>86</v>
+        <v>149</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>87</v>
+        <v>150</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>90</v>
+        <v>154</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>93</v>
+        <v>157</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>94</v>
+        <v>158</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>95</v>
+        <v>159</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>96</v>
+        <v>160</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>97</v>
+        <v>161</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>101</v>
+        <v>163</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>104</v>
+        <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>107</v>
+        <v>168</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>109</v>
+        <v>170</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>110</v>
+        <v>171</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>111</v>
+        <v>172</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>112</v>
+        <v>173</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>113</v>
+        <v>174</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>114</v>
+        <v>175</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>115</v>
+        <v>176</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>116</v>
+        <v>177</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>118</v>
+        <v>179</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>120</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>121</v>
+        <v>182</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>122</v>
+        <v>183</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>123</v>
+        <v>184</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>124</v>
+        <v>185</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>126</v>
+        <v>187</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>127</v>
+        <v>172</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>128</v>
+        <v>188</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>130</v>
+        <v>189</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>132</v>
+        <v>177</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>136</v>
+        <v>181</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>137</v>
+        <v>193</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>138</v>
+        <v>194</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>107</v>
+        <v>195</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>139</v>
+        <v>196</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>140</v>
+        <v>197</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>142</v>
+        <v>198</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>143</v>
+        <v>199</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>145</v>
+        <v>201</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>146</v>
+        <v>202</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>147</v>
+        <v>203</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>148</v>
+        <v>204</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>149</v>
+        <v>205</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>150</v>
+        <v>206</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>151</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>152</v>
+        <v>208</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>138</v>
+        <v>209</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>107</v>
+        <v>210</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>139</v>
+        <v>211</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>140</v>
+        <v>212</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>141</v>
+        <v>213</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>142</v>
+        <v>214</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>143</v>
+        <v>215</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>144</v>
+        <v>216</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>146</v>
+        <v>218</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>148</v>
+        <v>220</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>149</v>
+        <v>221</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>150</v>
+        <v>222</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>153</v>
+        <v>224</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>154</v>
+        <v>225</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>155</v>
+        <v>226</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>156</v>
+        <v>227</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>157</v>
+        <v>228</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>158</v>
+        <v>229</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>160</v>
+        <v>230</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>161</v>
+        <v>231</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>131</v>
+        <v>232</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>146</v>
+        <v>233</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>163</v>
+        <v>234</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>164</v>
+        <v>235</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>165</v>
+        <v>236</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="P22" s="2" t="s">
         <v>237</v>
       </c>
     </row>

</xml_diff>